<commit_message>
now, npm start working
</commit_message>
<xml_diff>
--- a/closingPricesAndHoldingsPAndL.xlsx
+++ b/closingPricesAndHoldingsPAndL.xlsx
@@ -424,10 +424,10 @@
         <v>485.36</v>
       </c>
       <c r="C2">
-        <v>512.14</v>
+        <v>540.11</v>
       </c>
       <c r="D2" t="str">
-        <v>5.52%</v>
+        <v>11.28%</v>
       </c>
     </row>
     <row r="3">
@@ -438,10 +438,10 @@
         <v>53.7</v>
       </c>
       <c r="C3">
-        <v>60.6</v>
+        <v>60.32</v>
       </c>
       <c r="D3" t="str">
-        <v>12.85%</v>
+        <v>12.33%</v>
       </c>
     </row>
     <row r="4">
@@ -452,10 +452,10 @@
         <v>654.44</v>
       </c>
       <c r="C4">
-        <v>764.4</v>
+        <v>759.09</v>
       </c>
       <c r="D4" t="str">
-        <v>16.8%</v>
+        <v>15.99%</v>
       </c>
     </row>
     <row r="5">
@@ -466,10 +466,10 @@
         <v>187.59</v>
       </c>
       <c r="C5">
-        <v>212.23</v>
+        <v>212.69</v>
       </c>
       <c r="D5" t="str">
-        <v>13.14%</v>
+        <v>13.38%</v>
       </c>
     </row>
     <row r="6">
@@ -480,10 +480,10 @@
         <v>246.76</v>
       </c>
       <c r="C6">
-        <v>260.65</v>
+        <v>266.95</v>
       </c>
       <c r="D6" t="str">
-        <v>5.63%</v>
+        <v>8.18%</v>
       </c>
     </row>
     <row r="7">
@@ -494,10 +494,10 @@
         <v>76.67</v>
       </c>
       <c r="C7">
-        <v>86.11</v>
+        <v>85.06</v>
       </c>
       <c r="D7" t="str">
-        <v>12.31%</v>
+        <v>10.94%</v>
       </c>
     </row>
   </sheetData>

</xml_diff>